<commit_message>
Add http://purl.obolibrary.org/obo/OBI_0000834 in the subset
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="597">
   <si>
     <t>planned process</t>
   </si>
@@ -1798,6 +1798,15 @@
   </si>
   <si>
     <t>biological_process</t>
+  </si>
+  <si>
+    <t>genomic_DNA</t>
+  </si>
+  <si>
+    <t>high molecular weight DNA extract</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000834</t>
   </si>
 </sst>
 </file>
@@ -1854,12 +1863,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2154,10 +2164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C210" sqref="C210"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2188,541 +2198,514 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>575</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>576</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D2" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>580</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>579</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D3" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>587</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>364</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>586</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>583</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>584</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>588</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>589</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>590</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>591</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>592</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>593</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>582</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>581</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D30" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D32" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>574</v>
@@ -2731,1830 +2714,1845 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>596</v>
+      </c>
+      <c r="B42" t="s">
+        <v>595</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="D42" t="s">
-        <v>112</v>
+      <c r="D42" s="5" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15">
       <c r="A52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" t="s">
-        <v>143</v>
+        <v>114</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D55" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D56" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>165</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>164</v>
+        <v>135</v>
+      </c>
+      <c r="B59" t="s">
+        <v>134</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D60" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B62" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D62" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D63" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D64" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="B65" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D66" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>192</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D68" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15">
       <c r="A69" t="s">
-        <v>195</v>
-      </c>
-      <c r="B69" t="s">
-        <v>194</v>
+        <v>165</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B70" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D70" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D71" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D73" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D74" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D75" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D76" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D77" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15">
       <c r="A78" t="s">
-        <v>222</v>
-      </c>
-      <c r="B78" t="s">
-        <v>221</v>
-      </c>
-      <c r="C78" t="s">
+        <v>192</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D78" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="B79" t="s">
-        <v>224</v>
-      </c>
-      <c r="C79" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D79" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D80" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="B81" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D81" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
-        <v>232</v>
-      </c>
-      <c r="C82" t="s">
+        <v>203</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D82" t="s">
-        <v>565</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="B83" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D83" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="B84" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D84" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="B85" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D85" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="B86" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D86" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D87" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="B88" t="s">
-        <v>250</v>
-      </c>
-      <c r="C88" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C88" t="s">
         <v>574</v>
       </c>
       <c r="D88" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="B89" t="s">
-        <v>253</v>
-      </c>
-      <c r="C89" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C89" t="s">
         <v>574</v>
       </c>
       <c r="D89" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="B90" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D90" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>260</v>
+        <v>231</v>
       </c>
       <c r="B91" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D91" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="B92" t="s">
-        <v>262</v>
-      </c>
-      <c r="C92" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C92" t="s">
         <v>574</v>
       </c>
       <c r="D92" t="s">
-        <v>261</v>
+        <v>565</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="B93" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D93" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D94" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="B95" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D95" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="B96" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D96" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="B97" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D97" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D98" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="B99" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D99" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="B100" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D100" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="B101" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D101" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
       <c r="B102" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D102" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="B103" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D103" t="s">
-        <v>292</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="B104" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D104" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="B105" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D105" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>302</v>
+        <v>274</v>
       </c>
       <c r="B106" t="s">
-        <v>301</v>
+        <v>273</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D106" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="B107" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D107" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="B108" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D108" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="B109" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D109" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
       <c r="B110" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D110" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="B111" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D111" t="s">
-        <v>566</v>
+        <v>286</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
       <c r="B112" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D112" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
       <c r="B113" t="s">
-        <v>321</v>
+        <v>293</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D113" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
       <c r="B114" t="s">
-        <v>324</v>
+        <v>296</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D114" t="s">
-        <v>323</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="B115" t="s">
-        <v>327</v>
+        <v>299</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D115" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="B116" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D116" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="B117" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D117" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="B118" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D118" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="B119" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D119" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>342</v>
+        <v>314</v>
       </c>
       <c r="B120" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D120" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="B121" t="s">
-        <v>344</v>
-      </c>
-      <c r="C121" t="s">
+        <v>315</v>
+      </c>
+      <c r="C121" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D121" t="s">
-        <v>343</v>
+        <v>566</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="B122" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D122" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
       <c r="B123" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D123" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="B124" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D124" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="B125" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D125" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="B126" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D126" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="B127" t="s">
-        <v>362</v>
+        <v>333</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D127" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="B128" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D128" t="s">
-        <v>364</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="B129" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D129" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>372</v>
+        <v>342</v>
       </c>
       <c r="B130" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D130" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>375</v>
+        <v>345</v>
       </c>
       <c r="B131" t="s">
-        <v>374</v>
-      </c>
-      <c r="C131" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C131" t="s">
         <v>574</v>
       </c>
       <c r="D131" t="s">
-        <v>373</v>
+        <v>343</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>378</v>
+        <v>348</v>
       </c>
       <c r="B132" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D132" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="B133" t="s">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D133" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
       <c r="B134" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D134" t="s">
-        <v>382</v>
+        <v>352</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
       <c r="B135" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D135" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="B136" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D136" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>392</v>
+        <v>363</v>
       </c>
       <c r="B137" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D137" t="s">
-        <v>390</v>
+        <v>361</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>395</v>
+        <v>366</v>
       </c>
       <c r="B138" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D138" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>398</v>
+        <v>369</v>
       </c>
       <c r="B139" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D139" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="15">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>400</v>
+        <v>372</v>
       </c>
       <c r="B140" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>567</v>
+      <c r="D140" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>402</v>
+        <v>375</v>
       </c>
       <c r="B141" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D141" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="B142" t="s">
-        <v>404</v>
+        <v>377</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D142" t="s">
-        <v>403</v>
+        <v>376</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="B143" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D143" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="B144" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D144" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="B145" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D145" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
       <c r="B146" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D146" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
       <c r="B147" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D147" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="B148" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D148" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>424</v>
+        <v>398</v>
       </c>
       <c r="B149" t="s">
-        <v>423</v>
+        <v>397</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D149" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15">
       <c r="A150" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="B150" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="D150" t="s">
-        <v>425</v>
+      <c r="D150" s="2" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>430</v>
+        <v>402</v>
       </c>
       <c r="B151" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D151" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>433</v>
+        <v>405</v>
       </c>
       <c r="B152" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D152" t="s">
-        <v>431</v>
+        <v>403</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>436</v>
+        <v>408</v>
       </c>
       <c r="B153" t="s">
-        <v>435</v>
+        <v>407</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D153" t="s">
-        <v>434</v>
+        <v>406</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>439</v>
+        <v>411</v>
       </c>
       <c r="B154" t="s">
-        <v>438</v>
+        <v>410</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D154" t="s">
-        <v>437</v>
+        <v>409</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="B155" t="s">
-        <v>441</v>
+        <v>413</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D155" t="s">
-        <v>440</v>
+        <v>412</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>445</v>
+        <v>414</v>
       </c>
       <c r="B156" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D156" t="s">
-        <v>443</v>
+        <v>415</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>448</v>
+        <v>418</v>
       </c>
       <c r="B157" t="s">
-        <v>447</v>
+        <v>417</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D157" t="s">
-        <v>446</v>
+        <v>416</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>451</v>
+        <v>421</v>
       </c>
       <c r="B158" t="s">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D158" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
       <c r="B159" t="s">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D159" t="s">
-        <v>452</v>
+        <v>422</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>457</v>
+        <v>427</v>
       </c>
       <c r="B160" t="s">
-        <v>456</v>
-      </c>
-      <c r="C160" t="s">
+        <v>426</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D160" t="s">
-        <v>455</v>
+        <v>425</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>460</v>
+        <v>430</v>
       </c>
       <c r="B161" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D161" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>463</v>
+        <v>433</v>
       </c>
       <c r="B162" t="s">
-        <v>462</v>
+        <v>432</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D162" t="s">
-        <v>461</v>
+        <v>431</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="B163" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D163" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>468</v>
+        <v>439</v>
       </c>
       <c r="B164" t="s">
-        <v>467</v>
+        <v>438</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D164" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>470</v>
+        <v>442</v>
       </c>
       <c r="B165" t="s">
-        <v>469</v>
+        <v>441</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D165" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>472</v>
+        <v>445</v>
       </c>
       <c r="B166" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D166" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>475</v>
+        <v>448</v>
       </c>
       <c r="B167" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D167" t="s">
-        <v>473</v>
+        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="B168" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D168" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="B169" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D169" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="B170" t="s">
-        <v>482</v>
-      </c>
-      <c r="C170" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C170" t="s">
         <v>574</v>
       </c>
       <c r="D170" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="B171" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D171" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="B172" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D172" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>491</v>
+        <v>466</v>
       </c>
       <c r="B173" t="s">
-        <v>490</v>
+        <v>465</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D173" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>493</v>
+        <v>468</v>
       </c>
       <c r="B174" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>574</v>
@@ -4562,382 +4560,382 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="B175" t="s">
-        <v>495</v>
+        <v>469</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D175" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>498</v>
+        <v>472</v>
       </c>
       <c r="B176" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D176" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>501</v>
+        <v>475</v>
       </c>
       <c r="B177" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D177" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="B178" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D178" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="B179" t="s">
-        <v>505</v>
+        <v>479</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D179" t="s">
-        <v>568</v>
+        <v>478</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="B180" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D180" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>512</v>
+        <v>486</v>
       </c>
       <c r="B181" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D181" t="s">
-        <v>510</v>
+        <v>484</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>515</v>
+        <v>489</v>
       </c>
       <c r="B182" t="s">
-        <v>514</v>
+        <v>488</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D182" t="s">
-        <v>513</v>
+        <v>487</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="B183" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D183" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
       <c r="B184" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D184" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
       <c r="B185" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D185" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="B186" t="s">
-        <v>526</v>
+        <v>497</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D186" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="B187" t="s">
-        <v>528</v>
+        <v>500</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D187" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
       <c r="B188" t="s">
-        <v>531</v>
+        <v>503</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D188" t="s">
-        <v>530</v>
+        <v>502</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
       <c r="B189" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D189" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="15">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
       <c r="B190" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="D190" s="1"/>
+      <c r="D190" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
       <c r="B191" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D191" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
       <c r="B192" t="s">
-        <v>542</v>
+        <v>514</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D192" t="s">
-        <v>541</v>
+        <v>513</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="B193" t="s">
-        <v>544</v>
+        <v>517</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D193" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>547</v>
+        <v>521</v>
       </c>
       <c r="B194" t="s">
-        <v>546</v>
+        <v>520</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D194" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B195" t="s">
-        <v>549</v>
+        <v>523</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D195" t="s">
-        <v>548</v>
+        <v>522</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="B196" t="s">
-        <v>552</v>
+        <v>526</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D196" t="s">
-        <v>551</v>
+        <v>525</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>556</v>
+        <v>529</v>
       </c>
       <c r="B197" t="s">
-        <v>555</v>
+        <v>528</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="D197" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>559</v>
+        <v>532</v>
       </c>
       <c r="B198" t="s">
-        <v>558</v>
+        <v>531</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D198" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" ht="15">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>562</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>561</v>
+        <v>535</v>
+      </c>
+      <c r="B199" t="s">
+        <v>534</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>574</v>
       </c>
       <c r="D199" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="15">
       <c r="A200" t="s">
-        <v>575</v>
+        <v>537</v>
       </c>
       <c r="B200" t="s">
-        <v>576</v>
+        <v>536</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>574</v>
       </c>
+      <c r="D200" s="1"/>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>577</v>
+        <v>540</v>
       </c>
       <c r="B201" t="s">
-        <v>578</v>
+        <v>539</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D201" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>580</v>
+        <v>543</v>
       </c>
       <c r="B202" t="s">
-        <v>579</v>
+        <v>542</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D202" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>582</v>
+        <v>545</v>
       </c>
       <c r="B203" t="s">
-        <v>581</v>
+        <v>544</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>574</v>
@@ -4945,10 +4943,10 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>583</v>
+        <v>547</v>
       </c>
       <c r="B204" t="s">
-        <v>584</v>
+        <v>546</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>574</v>
@@ -4956,60 +4954,89 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>585</v>
+        <v>550</v>
       </c>
       <c r="B205" t="s">
-        <v>586</v>
+        <v>549</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D205" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>587</v>
+        <v>553</v>
       </c>
       <c r="B206" t="s">
-        <v>364</v>
+        <v>552</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D206" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>588</v>
+        <v>556</v>
       </c>
       <c r="B207" t="s">
-        <v>589</v>
+        <v>555</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>574</v>
+      </c>
+      <c r="D207" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>590</v>
+        <v>559</v>
       </c>
       <c r="B208" t="s">
-        <v>591</v>
+        <v>558</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="209" spans="1:3">
+      <c r="D208" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="15">
       <c r="A209" t="s">
-        <v>592</v>
-      </c>
-      <c r="B209" t="s">
-        <v>593</v>
+        <v>562</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>574</v>
       </c>
+      <c r="D209" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" t="s">
+        <v>577</v>
+      </c>
+      <c r="B210" t="s">
+        <v>578</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>574</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E210">
+    <sortCondition ref="A2:A210"/>
+  </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Add Sequencing assay and its subclasses in the OBI subset Updated all the relevant files related to this change
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="25320" windowHeight="13545"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="601">
   <si>
     <t>planned process</t>
   </si>
@@ -1807,6 +1807,18 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0000834</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0600047</t>
+  </si>
+  <si>
+    <t>sequencing assay</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000010</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1880,7 +1892,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2164,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="A215" sqref="A215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5008,7 +5020,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15">
+    <row r="209" spans="1:5" ht="15">
       <c r="A209" t="s">
         <v>562</v>
       </c>
@@ -5022,7 +5034,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>577</v>
       </c>
@@ -5030,6 +5042,31 @@
         <v>578</v>
       </c>
       <c r="C210" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" t="s">
+        <v>597</v>
+      </c>
+      <c r="B211" t="s">
+        <v>598</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="E211" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" t="s">
+        <v>600</v>
+      </c>
+      <c r="B212" t="s">
+        <v>599</v>
+      </c>
+      <c r="C212" s="4" t="s">
         <v>574</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import OBI "differential expression analysis data transformation" (OBI_0000650)
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="601">
   <si>
     <t>planned process</t>
   </si>
@@ -2176,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="C216" sqref="C216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5067,6 +5067,17 @@
         <v>599</v>
       </c>
       <c r="C212" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" t="s">
+        <v>67</v>
+      </c>
+      <c r="B213" t="s">
+        <v>66</v>
+      </c>
+      <c r="C213" s="4" t="s">
         <v>574</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Import more terms for representation of GBCO data in RDF format
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15" windowWidth="20730" windowHeight="11760"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="606">
   <si>
     <t>planned process</t>
   </si>
@@ -1236,15 +1236,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0100051</t>
   </si>
   <si>
-    <t>CellLine</t>
-  </si>
-  <si>
-    <t>immortalized cell line culture</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0100056</t>
-  </si>
-  <si>
     <t>Transformation</t>
   </si>
   <si>
@@ -1819,13 +1810,37 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/IAO_0000010</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000429</t>
+  </si>
+  <si>
+    <t>email address</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000846</t>
+  </si>
+  <si>
+    <t>is member of organization</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001617</t>
+  </si>
+  <si>
+    <t>PubMed ID</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0009828</t>
+  </si>
+  <si>
+    <t>immortal cell line</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1854,6 +1869,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1875,24 +1895,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1966,6 +1992,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2000,6 +2027,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2175,14 +2203,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.28515625" customWidth="1"/>
     <col min="2" max="2" width="54.5703125" customWidth="1"/>
@@ -2191,123 +2219,123 @@
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>572</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>575</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>577</v>
+      </c>
+      <c r="B3" t="s">
         <v>576</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>580</v>
-      </c>
-      <c r="B3" t="s">
-        <v>579</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B4" t="s">
         <v>364</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B6" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>585</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>586</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>583</v>
-      </c>
-      <c r="B6" t="s">
-        <v>584</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="C7" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>587</v>
+      </c>
+      <c r="B8" t="s">
         <v>588</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>589</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>590</v>
       </c>
-      <c r="B8" t="s">
-        <v>591</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>592</v>
-      </c>
-      <c r="B9" t="s">
-        <v>593</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B10" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2315,13 +2343,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D11" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2329,13 +2357,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D12" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2343,13 +2371,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2357,13 +2385,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2371,13 +2399,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2385,13 +2413,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2399,13 +2427,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2413,13 +2441,13 @@
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2427,13 +2455,13 @@
         <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2441,13 +2469,13 @@
         <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2455,13 +2483,13 @@
         <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2469,13 +2497,13 @@
         <v>32</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2483,13 +2511,13 @@
         <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2497,10 +2525,10 @@
         <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2508,13 +2536,13 @@
         <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2522,10 +2550,10 @@
         <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -2533,13 +2561,13 @@
         <v>45</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2547,13 +2575,13 @@
         <v>48</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -2561,13 +2589,13 @@
         <v>51</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2575,10 +2603,10 @@
         <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -2586,10 +2614,10 @@
         <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2597,10 +2625,10 @@
         <v>57</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2608,13 +2636,13 @@
         <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2622,13 +2650,13 @@
         <v>63</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2636,13 +2664,13 @@
         <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -2650,13 +2678,13 @@
         <v>69</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2664,13 +2692,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -2678,13 +2706,13 @@
         <v>75</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -2692,13 +2720,13 @@
         <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -2706,13 +2734,13 @@
         <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D40" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2720,27 +2748,27 @@
         <v>84</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B42" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2748,13 +2776,13 @@
         <v>87</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D43" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2762,13 +2790,13 @@
         <v>90</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2776,13 +2804,13 @@
         <v>93</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2790,13 +2818,13 @@
         <v>96</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -2804,13 +2832,13 @@
         <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D47" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -2818,13 +2846,13 @@
         <v>102</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D48" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -2832,13 +2860,13 @@
         <v>105</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D49" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -2846,13 +2874,13 @@
         <v>108</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D50" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2860,13 +2888,13 @@
         <v>110</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15">
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -2874,13 +2902,13 @@
         <v>113</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -2888,13 +2916,13 @@
         <v>116</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D53" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>120</v>
       </c>
@@ -2902,13 +2930,13 @@
         <v>119</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D54" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -2916,13 +2944,13 @@
         <v>122</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>126</v>
       </c>
@@ -2930,13 +2958,13 @@
         <v>125</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D56" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>129</v>
       </c>
@@ -2944,13 +2972,13 @@
         <v>128</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D57" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -2958,13 +2986,13 @@
         <v>131</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D58" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -2972,13 +3000,13 @@
         <v>134</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D59" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>138</v>
       </c>
@@ -2986,13 +3014,13 @@
         <v>137</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D60" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -3000,13 +3028,13 @@
         <v>140</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D61" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -3014,13 +3042,13 @@
         <v>143</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D62" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>147</v>
       </c>
@@ -3028,13 +3056,13 @@
         <v>146</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>150</v>
       </c>
@@ -3042,13 +3070,13 @@
         <v>149</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D64" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -3056,13 +3084,13 @@
         <v>152</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D65" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -3070,13 +3098,13 @@
         <v>155</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D66" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>159</v>
       </c>
@@ -3084,13 +3112,13 @@
         <v>158</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D67" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>162</v>
       </c>
@@ -3098,13 +3126,13 @@
         <v>161</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D68" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15">
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>165</v>
       </c>
@@ -3112,13 +3140,13 @@
         <v>164</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D69" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>168</v>
       </c>
@@ -3126,13 +3154,13 @@
         <v>167</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D70" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>171</v>
       </c>
@@ -3140,13 +3168,13 @@
         <v>170</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D71" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>174</v>
       </c>
@@ -3154,13 +3182,13 @@
         <v>173</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D72" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -3168,13 +3196,13 @@
         <v>176</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D73" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>180</v>
       </c>
@@ -3182,13 +3210,13 @@
         <v>179</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D74" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>183</v>
       </c>
@@ -3196,13 +3224,13 @@
         <v>182</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D75" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>186</v>
       </c>
@@ -3210,13 +3238,13 @@
         <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D76" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>189</v>
       </c>
@@ -3224,13 +3252,13 @@
         <v>188</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D77" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15">
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>192</v>
       </c>
@@ -3238,13 +3266,13 @@
         <v>191</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D78" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>195</v>
       </c>
@@ -3252,13 +3280,13 @@
         <v>194</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D79" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -3266,13 +3294,13 @@
         <v>197</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D80" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>201</v>
       </c>
@@ -3280,13 +3308,13 @@
         <v>200</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D81" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>204</v>
       </c>
@@ -3294,13 +3322,13 @@
         <v>203</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D82" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -3308,13 +3336,13 @@
         <v>206</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D83" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>210</v>
       </c>
@@ -3322,13 +3350,13 @@
         <v>209</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D84" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>213</v>
       </c>
@@ -3336,13 +3364,13 @@
         <v>212</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D85" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>216</v>
       </c>
@@ -3350,13 +3378,13 @@
         <v>215</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D86" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>219</v>
       </c>
@@ -3364,13 +3392,13 @@
         <v>218</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D87" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>222</v>
       </c>
@@ -3378,13 +3406,13 @@
         <v>221</v>
       </c>
       <c r="C88" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D88" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>225</v>
       </c>
@@ -3392,13 +3420,13 @@
         <v>224</v>
       </c>
       <c r="C89" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D89" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>228</v>
       </c>
@@ -3406,13 +3434,13 @@
         <v>227</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D90" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>231</v>
       </c>
@@ -3420,13 +3448,13 @@
         <v>230</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D91" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>233</v>
       </c>
@@ -3434,13 +3462,13 @@
         <v>232</v>
       </c>
       <c r="C92" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D92" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>236</v>
       </c>
@@ -3448,13 +3476,13 @@
         <v>235</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D93" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>239</v>
       </c>
@@ -3462,13 +3490,13 @@
         <v>238</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D94" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>242</v>
       </c>
@@ -3476,13 +3504,13 @@
         <v>241</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D95" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>245</v>
       </c>
@@ -3490,13 +3518,13 @@
         <v>244</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D96" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>248</v>
       </c>
@@ -3504,13 +3532,13 @@
         <v>247</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D97" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>251</v>
       </c>
@@ -3518,13 +3546,13 @@
         <v>250</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D98" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>254</v>
       </c>
@@ -3532,13 +3560,13 @@
         <v>253</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D99" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>257</v>
       </c>
@@ -3546,13 +3574,13 @@
         <v>256</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D100" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>260</v>
       </c>
@@ -3560,13 +3588,13 @@
         <v>259</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D101" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>263</v>
       </c>
@@ -3574,13 +3602,13 @@
         <v>262</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D102" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>266</v>
       </c>
@@ -3588,13 +3616,13 @@
         <v>265</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D103" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>269</v>
       </c>
@@ -3602,13 +3630,13 @@
         <v>268</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D104" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>271</v>
       </c>
@@ -3616,10 +3644,10 @@
         <v>270</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>274</v>
       </c>
@@ -3627,13 +3655,13 @@
         <v>273</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D106" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>277</v>
       </c>
@@ -3641,13 +3669,13 @@
         <v>276</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D107" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>280</v>
       </c>
@@ -3655,13 +3683,13 @@
         <v>279</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D108" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>282</v>
       </c>
@@ -3669,10 +3697,10 @@
         <v>281</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>285</v>
       </c>
@@ -3680,13 +3708,13 @@
         <v>284</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D110" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>288</v>
       </c>
@@ -3694,13 +3722,13 @@
         <v>287</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D111" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>291</v>
       </c>
@@ -3708,13 +3736,13 @@
         <v>290</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D112" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>294</v>
       </c>
@@ -3722,13 +3750,13 @@
         <v>293</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D113" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>297</v>
       </c>
@@ -3736,13 +3764,13 @@
         <v>296</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D114" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>300</v>
       </c>
@@ -3750,13 +3778,13 @@
         <v>299</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D115" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>302</v>
       </c>
@@ -3764,10 +3792,10 @@
         <v>301</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>305</v>
       </c>
@@ -3775,13 +3803,13 @@
         <v>304</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D117" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>308</v>
       </c>
@@ -3789,13 +3817,13 @@
         <v>307</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D118" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>311</v>
       </c>
@@ -3803,13 +3831,13 @@
         <v>310</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D119" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>314</v>
       </c>
@@ -3817,13 +3845,13 @@
         <v>313</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D120" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>316</v>
       </c>
@@ -3831,13 +3859,13 @@
         <v>315</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D121" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>319</v>
       </c>
@@ -3845,13 +3873,13 @@
         <v>318</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D122" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>322</v>
       </c>
@@ -3859,13 +3887,13 @@
         <v>321</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D123" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>325</v>
       </c>
@@ -3873,13 +3901,13 @@
         <v>324</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D124" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>328</v>
       </c>
@@ -3887,13 +3915,13 @@
         <v>327</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D125" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>331</v>
       </c>
@@ -3901,13 +3929,13 @@
         <v>330</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D126" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>334</v>
       </c>
@@ -3915,13 +3943,13 @@
         <v>333</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D127" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>337</v>
       </c>
@@ -3929,13 +3957,13 @@
         <v>336</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D128" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>340</v>
       </c>
@@ -3943,13 +3971,13 @@
         <v>339</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D129" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>342</v>
       </c>
@@ -3957,10 +3985,10 @@
         <v>341</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>345</v>
       </c>
@@ -3968,13 +3996,13 @@
         <v>344</v>
       </c>
       <c r="C131" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D131" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>348</v>
       </c>
@@ -3982,13 +4010,13 @@
         <v>347</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D132" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>351</v>
       </c>
@@ -3996,13 +4024,13 @@
         <v>350</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D133" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>354</v>
       </c>
@@ -4010,13 +4038,13 @@
         <v>353</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D134" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>357</v>
       </c>
@@ -4024,13 +4052,13 @@
         <v>356</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D135" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>360</v>
       </c>
@@ -4038,13 +4066,13 @@
         <v>359</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D136" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>363</v>
       </c>
@@ -4052,13 +4080,13 @@
         <v>362</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D137" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>366</v>
       </c>
@@ -4066,13 +4094,13 @@
         <v>365</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D138" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>369</v>
       </c>
@@ -4080,13 +4108,13 @@
         <v>368</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D139" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>372</v>
       </c>
@@ -4094,13 +4122,13 @@
         <v>371</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D140" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>375</v>
       </c>
@@ -4108,13 +4136,13 @@
         <v>374</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D141" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>378</v>
       </c>
@@ -4122,13 +4150,13 @@
         <v>377</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D142" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>381</v>
       </c>
@@ -4136,13 +4164,13 @@
         <v>380</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D143" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>384</v>
       </c>
@@ -4150,13 +4178,13 @@
         <v>383</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D144" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>387</v>
       </c>
@@ -4164,13 +4192,13 @@
         <v>386</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D145" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>389</v>
       </c>
@@ -4178,10 +4206,10 @@
         <v>388</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>392</v>
       </c>
@@ -4189,13 +4217,13 @@
         <v>391</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D147" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>395</v>
       </c>
@@ -4203,13 +4231,13 @@
         <v>394</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D148" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>398</v>
       </c>
@@ -4217,13 +4245,13 @@
         <v>397</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D149" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15">
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>400</v>
       </c>
@@ -4231,13 +4259,13 @@
         <v>399</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>402</v>
       </c>
@@ -4245,13 +4273,13 @@
         <v>401</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D151" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>405</v>
       </c>
@@ -4259,13 +4287,13 @@
         <v>404</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D152" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>408</v>
       </c>
@@ -4273,13 +4301,13 @@
         <v>407</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D153" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>411</v>
       </c>
@@ -4287,41 +4315,41 @@
         <v>410</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D154" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B155" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D155" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>415</v>
+      </c>
+      <c r="B156" t="s">
         <v>414</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D156" t="s">
         <v>413</v>
       </c>
-      <c r="C156" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D156" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>418</v>
       </c>
@@ -4329,13 +4357,13 @@
         <v>417</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D157" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>421</v>
       </c>
@@ -4343,13 +4371,13 @@
         <v>420</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D158" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>424</v>
       </c>
@@ -4357,13 +4385,13 @@
         <v>423</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D159" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>427</v>
       </c>
@@ -4371,13 +4399,13 @@
         <v>426</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D160" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>430</v>
       </c>
@@ -4385,13 +4413,13 @@
         <v>429</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D161" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>433</v>
       </c>
@@ -4399,13 +4427,13 @@
         <v>432</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D162" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>436</v>
       </c>
@@ -4413,13 +4441,13 @@
         <v>435</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D163" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>439</v>
       </c>
@@ -4427,13 +4455,13 @@
         <v>438</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D164" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>442</v>
       </c>
@@ -4441,13 +4469,13 @@
         <v>441</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D165" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>445</v>
       </c>
@@ -4455,13 +4483,13 @@
         <v>444</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D166" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>448</v>
       </c>
@@ -4469,13 +4497,13 @@
         <v>447</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D167" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>451</v>
       </c>
@@ -4483,41 +4511,41 @@
         <v>450</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D168" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>454</v>
       </c>
       <c r="B169" t="s">
         <v>453</v>
       </c>
-      <c r="C169" s="4" t="s">
-        <v>574</v>
+      <c r="C169" t="s">
+        <v>571</v>
       </c>
       <c r="D169" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>457</v>
       </c>
       <c r="B170" t="s">
         <v>456</v>
       </c>
-      <c r="C170" t="s">
-        <v>574</v>
+      <c r="C170" s="4" t="s">
+        <v>571</v>
       </c>
       <c r="D170" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>460</v>
       </c>
@@ -4525,13 +4553,13 @@
         <v>459</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D171" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>463</v>
       </c>
@@ -4539,49 +4567,46 @@
         <v>462</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D172" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>465</v>
+      </c>
+      <c r="B173" t="s">
+        <v>464</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>467</v>
+      </c>
+      <c r="B174" t="s">
         <v>466</v>
       </c>
-      <c r="B173" t="s">
-        <v>465</v>
-      </c>
-      <c r="C173" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D173" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174" t="s">
+      <c r="C174" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>469</v>
+      </c>
+      <c r="B175" t="s">
         <v>468</v>
       </c>
-      <c r="B174" t="s">
-        <v>467</v>
-      </c>
-      <c r="C174" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
-      <c r="A175" t="s">
-        <v>470</v>
-      </c>
-      <c r="B175" t="s">
-        <v>469</v>
-      </c>
       <c r="C175" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>472</v>
       </c>
@@ -4589,24 +4614,24 @@
         <v>471</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D176" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B177" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D177" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>477</v>
       </c>
@@ -4614,10 +4639,13 @@
         <v>476</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D178" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>480</v>
       </c>
@@ -4625,13 +4653,13 @@
         <v>479</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D179" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>483</v>
       </c>
@@ -4639,13 +4667,13 @@
         <v>482</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D180" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>486</v>
       </c>
@@ -4653,38 +4681,35 @@
         <v>485</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D181" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>488</v>
+      </c>
+      <c r="B182" t="s">
+        <v>487</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>490</v>
+      </c>
+      <c r="B183" t="s">
         <v>489</v>
       </c>
-      <c r="B182" t="s">
-        <v>488</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D182" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="A183" t="s">
-        <v>491</v>
-      </c>
-      <c r="B183" t="s">
-        <v>490</v>
-      </c>
       <c r="C183" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>493</v>
       </c>
@@ -4692,24 +4717,27 @@
         <v>492</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D184" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B185" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D185" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>498</v>
       </c>
@@ -4717,13 +4745,13 @@
         <v>497</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D186" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>501</v>
       </c>
@@ -4731,27 +4759,27 @@
         <v>500</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D187" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B188" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D188" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>506</v>
       </c>
@@ -4759,13 +4787,13 @@
         <v>505</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D189" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>509</v>
       </c>
@@ -4773,13 +4801,13 @@
         <v>508</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D190" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>512</v>
       </c>
@@ -4787,13 +4815,13 @@
         <v>511</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D191" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>515</v>
       </c>
@@ -4801,13 +4829,13 @@
         <v>514</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D192" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>518</v>
       </c>
@@ -4815,13 +4843,13 @@
         <v>517</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D193" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>521</v>
       </c>
@@ -4829,13 +4857,13 @@
         <v>520</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D194" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>524</v>
       </c>
@@ -4843,27 +4871,24 @@
         <v>523</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D195" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B196" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D196" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>529</v>
       </c>
@@ -4871,10 +4896,13 @@
         <v>528</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D197" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>532</v>
       </c>
@@ -4882,27 +4910,25 @@
         <v>531</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D198" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B199" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D199" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" ht="15">
+        <v>571</v>
+      </c>
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>537</v>
       </c>
@@ -4910,11 +4936,13 @@
         <v>536</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D200" s="1"/>
-    </row>
-    <row r="201" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D200" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>540</v>
       </c>
@@ -4922,38 +4950,35 @@
         <v>539</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D201" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>542</v>
+      </c>
+      <c r="B202" t="s">
+        <v>541</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>544</v>
+      </c>
+      <c r="B203" t="s">
         <v>543</v>
       </c>
-      <c r="B202" t="s">
-        <v>542</v>
-      </c>
-      <c r="C202" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D202" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" t="s">
-        <v>545</v>
-      </c>
-      <c r="B203" t="s">
-        <v>544</v>
-      </c>
       <c r="C203" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>547</v>
       </c>
@@ -4961,10 +4986,13 @@
         <v>546</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
+        <v>571</v>
+      </c>
+      <c r="D204" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>550</v>
       </c>
@@ -4972,13 +5000,13 @@
         <v>549</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D205" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>553</v>
       </c>
@@ -4986,13 +5014,13 @@
         <v>552</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D206" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>556</v>
       </c>
@@ -5000,85 +5028,115 @@
         <v>555</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D207" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>559</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="2" t="s">
         <v>558</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D208" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="15">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>562</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>561</v>
+        <v>574</v>
+      </c>
+      <c r="B209" t="s">
+        <v>575</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D209" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>577</v>
+        <v>594</v>
       </c>
       <c r="B210" t="s">
-        <v>578</v>
+        <v>595</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5">
+        <v>571</v>
+      </c>
+      <c r="E210" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>597</v>
       </c>
       <c r="B211" t="s">
+        <v>596</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>67</v>
+      </c>
+      <c r="B212" t="s">
+        <v>66</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
         <v>598</v>
       </c>
-      <c r="C211" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="E211" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5">
-      <c r="A212" t="s">
+      <c r="B213" t="s">
+        <v>599</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
         <v>600</v>
       </c>
-      <c r="B212" t="s">
-        <v>599</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5">
-      <c r="A213" t="s">
-        <v>67</v>
-      </c>
-      <c r="B213" t="s">
-        <v>66</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>574</v>
+      <c r="B214" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>602</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>604</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -5092,12 +5150,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5106,12 +5164,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update OBI subset including all study design and related terms
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519" refMode="R1C1" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="608">
   <si>
     <t>planned process</t>
   </si>
@@ -1834,6 +1834,12 @@
   </si>
   <si>
     <t>immortal cell line</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000208</t>
+  </si>
+  <si>
+    <t>methodology testing objective</t>
   </si>
 </sst>
 </file>
@@ -2204,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="C220" sqref="C220"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D218" sqref="D218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4620,7 +4626,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>474</v>
       </c>
@@ -4631,7 +4637,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>477</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>480</v>
       </c>
@@ -4659,7 +4665,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>483</v>
       </c>
@@ -4673,7 +4679,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>486</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>488</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>490</v>
       </c>
@@ -4709,7 +4715,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>493</v>
       </c>
@@ -4723,7 +4729,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>495</v>
       </c>
@@ -4737,7 +4743,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>498</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>501</v>
       </c>
@@ -4765,7 +4771,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>503</v>
       </c>
@@ -4778,8 +4784,11 @@
       <c r="D188" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E188" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>506</v>
       </c>
@@ -4793,7 +4802,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>509</v>
       </c>
@@ -4807,7 +4816,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>512</v>
       </c>
@@ -4821,7 +4830,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>515</v>
       </c>
@@ -5136,6 +5145,20 @@
         <v>605</v>
       </c>
       <c r="C216" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>606</v>
+      </c>
+      <c r="B217" t="s">
+        <v>607</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="E217" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Import terms from OBO Foundry ontologies for Study properties and factor type annotation. More terms may need to be imported later.
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="638">
   <si>
     <t>planned process</t>
   </si>
@@ -1840,6 +1840,96 @@
   </si>
   <si>
     <t>methodology testing objective</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000181</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000424</t>
+  </si>
+  <si>
+    <t>transcription profiling assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001271</t>
+  </si>
+  <si>
+    <t>RNA-seq assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001361</t>
+  </si>
+  <si>
+    <t>transcription profiling by RT-PCR assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001463</t>
+  </si>
+  <si>
+    <t>transcription profiling by array assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001853</t>
+  </si>
+  <si>
+    <t>DNase I hypersensitive sites sequencing assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001859</t>
+  </si>
+  <si>
+    <t>formaldehyde-assisted isolation of regulatory elements assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002014</t>
+  </si>
+  <si>
+    <t>DNA methylation profiling by ChIP-chip assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002015</t>
+  </si>
+  <si>
+    <t>transcription profiling by MPSS assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002016</t>
+  </si>
+  <si>
+    <t>histone modification identification by ChIP-chip assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002017</t>
+  </si>
+  <si>
+    <t>histone modification identification by ChIP-Seq assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002018</t>
+  </si>
+  <si>
+    <t>transcription factor binding site identification by ChIP-chip assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002019</t>
+  </si>
+  <si>
+    <t>transcription factor binding site identification by ChIP-Seq assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002020</t>
+  </si>
+  <si>
+    <t>epigenetic modification assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002021</t>
+  </si>
+  <si>
+    <t>transcription factor binding site identification</t>
   </si>
 </sst>
 </file>
@@ -2210,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E217"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D218" sqref="D218"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2277,10 +2367,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>582</v>
-      </c>
-      <c r="B5" t="s">
-        <v>583</v>
+        <v>604</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>605</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>571</v>
@@ -2288,10 +2378,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B6" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>571</v>
@@ -2299,10 +2389,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="B7" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>571</v>
@@ -2310,10 +2400,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>571</v>
@@ -2321,10 +2411,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B9" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>571</v>
@@ -2332,10 +2422,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="B10" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>571</v>
@@ -2343,2555 +2433,2504 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>579</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>578</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D11" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>597</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>596</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D12" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>598</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>599</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C19" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C20" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C21" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>609</v>
+      </c>
+      <c r="B22" t="s">
+        <v>608</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C23" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C24" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C25" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>606</v>
+      </c>
+      <c r="B26" t="s">
+        <v>607</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="E26" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C27" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C28" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C29" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C30" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C31" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C32" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D32" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D35" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>610</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>611</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D37" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D38" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>593</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>592</v>
+        <v>66</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D45" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>593</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>592</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D49" t="s">
-        <v>104</v>
+      <c r="D49" s="5" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" t="s">
-        <v>108</v>
+        <v>600</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>601</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D52" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D58" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>138</v>
-      </c>
-      <c r="B60" t="s">
-        <v>137</v>
+        <v>114</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D60" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D61" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D64" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D65" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D66" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D67" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>165</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>164</v>
+        <v>141</v>
+      </c>
+      <c r="B69" t="s">
+        <v>140</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D69" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D70" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D71" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D72" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D73" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="B74" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D74" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D75" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D76" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>189</v>
-      </c>
-      <c r="B77" t="s">
-        <v>188</v>
+        <v>165</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D77" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>192</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>191</v>
+        <v>168</v>
+      </c>
+      <c r="B78" t="s">
+        <v>167</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D78" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D79" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D80" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="B81" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D81" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D82" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B83" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D83" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="B84" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="B85" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D85" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>216</v>
-      </c>
-      <c r="B86" t="s">
-        <v>215</v>
+        <v>192</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D86" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D87" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="B88" t="s">
-        <v>221</v>
-      </c>
-      <c r="C88" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D88" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="B89" t="s">
-        <v>224</v>
-      </c>
-      <c r="C89" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D89" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="B90" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D90" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="B91" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D91" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
-      </c>
-      <c r="C92" t="s">
+        <v>209</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D92" t="s">
-        <v>562</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="B93" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D93" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B94" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D94" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="B95" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D95" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B96" t="s">
-        <v>244</v>
-      </c>
-      <c r="C96" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C96" t="s">
         <v>571</v>
       </c>
       <c r="D96" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B97" t="s">
-        <v>247</v>
-      </c>
-      <c r="C97" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C97" t="s">
         <v>571</v>
       </c>
       <c r="D97" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B98" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D98" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="B99" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D99" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="B100" t="s">
-        <v>256</v>
-      </c>
-      <c r="C100" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C100" t="s">
         <v>571</v>
       </c>
       <c r="D100" t="s">
-        <v>255</v>
+        <v>562</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="B101" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D101" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B102" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D102" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="B103" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D103" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="B104" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D104" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="B105" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D105" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="B106" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D106" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="B107" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D107" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="B108" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D108" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D109" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>285</v>
+        <v>612</v>
       </c>
       <c r="B110" t="s">
-        <v>284</v>
+        <v>613</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D110" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="B111" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D111" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="B112" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D112" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B113" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D113" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="B114" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D114" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="B115" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D115" t="s">
-        <v>298</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="B116" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D116" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B117" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D117" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="B118" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D118" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
       <c r="B119" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D119" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="B120" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D120" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="B121" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D121" t="s">
-        <v>563</v>
+        <v>289</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D122" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="B123" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D123" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>325</v>
+        <v>614</v>
       </c>
       <c r="B124" t="s">
-        <v>324</v>
+        <v>615</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D124" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="B125" t="s">
-        <v>327</v>
+        <v>299</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D125" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="B126" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D126" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="B127" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D127" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="B128" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D128" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="B129" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D129" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>342</v>
+        <v>314</v>
       </c>
       <c r="B130" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D130" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="B131" t="s">
-        <v>344</v>
-      </c>
-      <c r="C131" t="s">
+        <v>315</v>
+      </c>
+      <c r="C131" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D131" t="s">
-        <v>343</v>
+        <v>563</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="B132" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D132" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
       <c r="B133" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D133" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="B134" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D134" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="B135" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D135" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="B136" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D136" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="B137" t="s">
-        <v>362</v>
+        <v>333</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D137" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="B138" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D138" t="s">
-        <v>364</v>
+        <v>335</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="B139" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D139" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>372</v>
+        <v>342</v>
       </c>
       <c r="B140" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D140" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>375</v>
+        <v>345</v>
       </c>
       <c r="B141" t="s">
-        <v>374</v>
-      </c>
-      <c r="C141" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C141" t="s">
         <v>571</v>
       </c>
       <c r="D141" t="s">
-        <v>373</v>
+        <v>343</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>378</v>
+        <v>348</v>
       </c>
       <c r="B142" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D142" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="B143" t="s">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D143" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
       <c r="B144" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D144" t="s">
-        <v>382</v>
+        <v>352</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
       <c r="B145" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D145" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="B146" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D146" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>392</v>
+        <v>616</v>
       </c>
       <c r="B147" t="s">
-        <v>391</v>
+        <v>617</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D147" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>395</v>
+        <v>363</v>
       </c>
       <c r="B148" t="s">
-        <v>394</v>
+        <v>362</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D148" t="s">
-        <v>393</v>
+        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>398</v>
+        <v>366</v>
       </c>
       <c r="B149" t="s">
-        <v>397</v>
+        <v>365</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D149" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="B150" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D150" s="2" t="s">
-        <v>564</v>
+      <c r="D150" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>402</v>
+        <v>372</v>
       </c>
       <c r="B151" t="s">
-        <v>401</v>
+        <v>371</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D151" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="B152" t="s">
-        <v>404</v>
+        <v>374</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D152" t="s">
-        <v>403</v>
+        <v>373</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="B153" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D153" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="B154" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D154" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="B155" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D155" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>415</v>
+        <v>387</v>
       </c>
       <c r="B156" t="s">
-        <v>414</v>
+        <v>386</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D156" t="s">
-        <v>413</v>
+        <v>385</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>418</v>
+        <v>389</v>
       </c>
       <c r="B157" t="s">
-        <v>417</v>
+        <v>388</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D157" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>421</v>
+        <v>392</v>
       </c>
       <c r="B158" t="s">
-        <v>420</v>
+        <v>391</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D158" t="s">
-        <v>419</v>
+        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>424</v>
+        <v>395</v>
       </c>
       <c r="B159" t="s">
-        <v>423</v>
+        <v>394</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D159" t="s">
-        <v>422</v>
+        <v>393</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>427</v>
+        <v>398</v>
       </c>
       <c r="B160" t="s">
-        <v>426</v>
+        <v>397</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D160" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="B161" t="s">
-        <v>429</v>
+        <v>399</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D161" t="s">
-        <v>428</v>
+      <c r="D161" s="2" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>433</v>
-      </c>
-      <c r="B162" t="s">
-        <v>432</v>
+        <v>602</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>603</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D162" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>436</v>
+        <v>618</v>
       </c>
       <c r="B163" t="s">
-        <v>435</v>
+        <v>619</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D163" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>439</v>
+        <v>620</v>
       </c>
       <c r="B164" t="s">
-        <v>438</v>
+        <v>621</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D164" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>442</v>
+        <v>622</v>
       </c>
       <c r="B165" t="s">
-        <v>441</v>
+        <v>623</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D165" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>445</v>
+        <v>624</v>
       </c>
       <c r="B166" t="s">
-        <v>444</v>
+        <v>625</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D166" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>448</v>
+        <v>626</v>
       </c>
       <c r="B167" t="s">
-        <v>447</v>
+        <v>627</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D167" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>451</v>
+        <v>628</v>
       </c>
       <c r="B168" t="s">
-        <v>450</v>
+        <v>629</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D168" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>454</v>
+        <v>630</v>
       </c>
       <c r="B169" t="s">
-        <v>453</v>
-      </c>
-      <c r="C169" t="s">
-        <v>571</v>
-      </c>
-      <c r="D169" t="s">
-        <v>452</v>
+        <v>631</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>457</v>
+        <v>632</v>
       </c>
       <c r="B170" t="s">
-        <v>456</v>
+        <v>633</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D170" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>460</v>
+        <v>634</v>
       </c>
       <c r="B171" t="s">
-        <v>459</v>
+        <v>635</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D171" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>463</v>
+        <v>636</v>
       </c>
       <c r="B172" t="s">
-        <v>462</v>
+        <v>637</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D172" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>465</v>
+        <v>402</v>
       </c>
       <c r="B173" t="s">
-        <v>464</v>
+        <v>401</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D173" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>467</v>
+        <v>405</v>
       </c>
       <c r="B174" t="s">
-        <v>466</v>
+        <v>404</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D174" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>469</v>
+        <v>408</v>
       </c>
       <c r="B175" t="s">
-        <v>468</v>
+        <v>407</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D175" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>472</v>
+        <v>411</v>
       </c>
       <c r="B176" t="s">
-        <v>471</v>
+        <v>410</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D176" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>474</v>
+        <v>411</v>
       </c>
       <c r="B177" t="s">
-        <v>473</v>
+        <v>410</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>477</v>
+        <v>415</v>
       </c>
       <c r="B178" t="s">
-        <v>476</v>
+        <v>414</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D178" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>480</v>
+        <v>418</v>
       </c>
       <c r="B179" t="s">
-        <v>479</v>
+        <v>417</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D179" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>483</v>
+        <v>421</v>
       </c>
       <c r="B180" t="s">
-        <v>482</v>
+        <v>420</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D180" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>486</v>
+        <v>424</v>
       </c>
       <c r="B181" t="s">
-        <v>485</v>
+        <v>423</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D181" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>488</v>
+        <v>427</v>
       </c>
       <c r="B182" t="s">
-        <v>487</v>
+        <v>426</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D182" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>490</v>
+        <v>430</v>
       </c>
       <c r="B183" t="s">
-        <v>489</v>
+        <v>429</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>493</v>
+        <v>433</v>
       </c>
       <c r="B184" t="s">
-        <v>492</v>
+        <v>432</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D184" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>495</v>
+        <v>436</v>
       </c>
       <c r="B185" t="s">
-        <v>494</v>
+        <v>435</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D185" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>498</v>
+        <v>439</v>
       </c>
       <c r="B186" t="s">
-        <v>497</v>
+        <v>438</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D186" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>501</v>
+        <v>442</v>
       </c>
       <c r="B187" t="s">
-        <v>500</v>
+        <v>441</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D187" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>503</v>
+        <v>445</v>
       </c>
       <c r="B188" t="s">
-        <v>502</v>
+        <v>444</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D188" t="s">
-        <v>565</v>
-      </c>
-      <c r="E188" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>506</v>
+        <v>448</v>
       </c>
       <c r="B189" t="s">
-        <v>505</v>
+        <v>447</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D189" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>509</v>
+        <v>451</v>
       </c>
       <c r="B190" t="s">
-        <v>508</v>
+        <v>450</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D190" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>512</v>
+        <v>454</v>
       </c>
       <c r="B191" t="s">
-        <v>511</v>
-      </c>
-      <c r="C191" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C191" t="s">
         <v>571</v>
       </c>
       <c r="D191" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>515</v>
+        <v>457</v>
       </c>
       <c r="B192" t="s">
-        <v>514</v>
+        <v>456</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D192" t="s">
-        <v>513</v>
+        <v>455</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>518</v>
+        <v>460</v>
       </c>
       <c r="B193" t="s">
-        <v>517</v>
+        <v>459</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D193" t="s">
-        <v>516</v>
+        <v>458</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>521</v>
+        <v>463</v>
       </c>
       <c r="B194" t="s">
-        <v>520</v>
+        <v>462</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D194" t="s">
-        <v>519</v>
+        <v>461</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>524</v>
+        <v>465</v>
       </c>
       <c r="B195" t="s">
-        <v>523</v>
+        <v>464</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D195" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>526</v>
+        <v>467</v>
       </c>
       <c r="B196" t="s">
-        <v>525</v>
+        <v>466</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>571</v>
@@ -4899,184 +4938,186 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>529</v>
+        <v>469</v>
       </c>
       <c r="B197" t="s">
-        <v>528</v>
+        <v>468</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D197" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>532</v>
+        <v>472</v>
       </c>
       <c r="B198" t="s">
-        <v>531</v>
+        <v>471</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D198" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>534</v>
+        <v>474</v>
       </c>
       <c r="B199" t="s">
-        <v>533</v>
+        <v>473</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D199" s="1"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>537</v>
+        <v>477</v>
       </c>
       <c r="B200" t="s">
-        <v>536</v>
+        <v>476</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D200" t="s">
-        <v>535</v>
+        <v>475</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="B201" t="s">
-        <v>539</v>
+        <v>479</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D201" t="s">
-        <v>538</v>
+        <v>478</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>542</v>
+        <v>483</v>
       </c>
       <c r="B202" t="s">
-        <v>541</v>
+        <v>482</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D202" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>544</v>
+        <v>486</v>
       </c>
       <c r="B203" t="s">
-        <v>543</v>
+        <v>485</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D203" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>547</v>
+        <v>488</v>
       </c>
       <c r="B204" t="s">
-        <v>546</v>
+        <v>487</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D204" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>550</v>
+        <v>490</v>
       </c>
       <c r="B205" t="s">
-        <v>549</v>
+        <v>489</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D205" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>553</v>
+        <v>493</v>
       </c>
       <c r="B206" t="s">
-        <v>552</v>
+        <v>492</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D206" t="s">
-        <v>551</v>
+        <v>491</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>556</v>
+        <v>495</v>
       </c>
       <c r="B207" t="s">
-        <v>555</v>
+        <v>494</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D207" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>559</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>558</v>
+        <v>498</v>
+      </c>
+      <c r="B208" t="s">
+        <v>497</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D208" t="s">
-        <v>557</v>
+        <v>496</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>574</v>
+        <v>501</v>
       </c>
       <c r="B209" t="s">
-        <v>575</v>
+        <v>500</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D209" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>594</v>
+        <v>503</v>
       </c>
       <c r="B210" t="s">
-        <v>595</v>
+        <v>502</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D210" t="s">
+        <v>565</v>
       </c>
       <c r="E210" t="s">
         <v>571</v>
@@ -5084,90 +5125,305 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>597</v>
+        <v>506</v>
       </c>
       <c r="B211" t="s">
-        <v>596</v>
+        <v>505</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D211" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>67</v>
+        <v>509</v>
       </c>
       <c r="B212" t="s">
-        <v>66</v>
+        <v>508</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D212" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>598</v>
+        <v>512</v>
       </c>
       <c r="B213" t="s">
-        <v>599</v>
+        <v>511</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D213" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>600</v>
-      </c>
-      <c r="B214" s="6" t="s">
-        <v>601</v>
+        <v>515</v>
+      </c>
+      <c r="B214" t="s">
+        <v>514</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D214" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>602</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>603</v>
+        <v>518</v>
+      </c>
+      <c r="B215" t="s">
+        <v>517</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D215" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>604</v>
-      </c>
-      <c r="B216" s="6" t="s">
-        <v>605</v>
+        <v>521</v>
+      </c>
+      <c r="B216" t="s">
+        <v>520</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D216" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>606</v>
+        <v>524</v>
       </c>
       <c r="B217" t="s">
-        <v>607</v>
+        <v>523</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="E217" t="s">
+      <c r="D217" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>526</v>
+      </c>
+      <c r="B218" t="s">
+        <v>525</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>529</v>
+      </c>
+      <c r="B219" t="s">
+        <v>528</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D219" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>532</v>
+      </c>
+      <c r="B220" t="s">
+        <v>531</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D220" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>534</v>
+      </c>
+      <c r="B221" t="s">
+        <v>533</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D221" s="1"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>537</v>
+      </c>
+      <c r="B222" t="s">
+        <v>536</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D222" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>540</v>
+      </c>
+      <c r="B223" t="s">
+        <v>539</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D223" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>542</v>
+      </c>
+      <c r="B224" t="s">
+        <v>541</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>544</v>
+      </c>
+      <c r="B225" t="s">
+        <v>543</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>547</v>
+      </c>
+      <c r="B226" t="s">
+        <v>546</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D226" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>594</v>
+      </c>
+      <c r="B227" t="s">
+        <v>595</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="E227" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>550</v>
+      </c>
+      <c r="B228" t="s">
+        <v>549</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D228" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>553</v>
+      </c>
+      <c r="B229" t="s">
+        <v>552</v>
+      </c>
+      <c r="C229" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D229" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>556</v>
+      </c>
+      <c r="B230" t="s">
+        <v>555</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D230" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>559</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C231" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D231" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>574</v>
+      </c>
+      <c r="B232" t="s">
+        <v>575</v>
+      </c>
+      <c r="C232" s="4" t="s">
         <v>571</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E210">
-    <sortCondition ref="A2:A210"/>
+  <sortState ref="A2:E233">
+    <sortCondition ref="A2:A233"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Import term 'bead' Generated OBI_subset.owl based on OBI_output.owl - removed annotations and axioms used to defined a term not in OBI and IAO. - replace PATO_0001237 by PATO_0002182 since this deprecated PATO term is used in OBI - manually added a few newly added assay terms which is not in the released OBI and cannot be retrieved by ontoDog
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="640">
   <si>
     <t>planned process</t>
   </si>
@@ -1930,6 +1930,12 @@
   </si>
   <si>
     <t>transcription factor binding site identification</t>
+  </si>
+  <si>
+    <t>bead</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_1000207</t>
   </si>
 </sst>
 </file>
@@ -2300,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="C237" sqref="C237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5380,40 +5386,51 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>639</v>
+      </c>
+      <c r="B230" t="s">
+        <v>638</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
         <v>556</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>555</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D230" t="s">
+      <c r="C231" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D231" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+    <row r="232" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>559</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B232" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D231" t="s">
+      <c r="C232" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D232" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
         <v>574</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>575</v>
       </c>
-      <c r="C232" s="4" t="s">
+      <c r="C233" s="4" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Import OBI term 'transcription factor binding site identification'
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="642">
   <si>
     <t>planned process</t>
   </si>
@@ -1936,6 +1936,12 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_1000207</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000291</t>
+  </si>
+  <si>
+    <t>transcription factor binding site  identification</t>
   </si>
 </sst>
 </file>
@@ -2306,10 +2312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="C237" sqref="C237"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2715,63 +2721,63 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>640</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>641</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>610</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>611</v>
+        <v>53</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>571</v>
@@ -2779,10 +2785,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>610</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>611</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>571</v>
@@ -2790,10 +2796,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>571</v>
@@ -2801,44 +2807,41 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D39" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2851,1663 +2854,1666 @@
       <c r="C42" s="4" t="s">
         <v>571</v>
       </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D43" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>593</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>592</v>
+        <v>84</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>591</v>
+      <c r="D49" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>600</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>601</v>
+        <v>593</v>
+      </c>
+      <c r="B50" t="s">
+        <v>592</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>87</v>
+        <v>600</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>601</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D51" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D52" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D57" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>111</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C60" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>114</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C61" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D61" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D61" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D62" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D63" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D64" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D66" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D68" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B69" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D69" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D70" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D73" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D74" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>162</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C77" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D77" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>165</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="C78" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D78" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>168</v>
-      </c>
-      <c r="B78" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D78" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D79" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B80" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D80" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D82" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B83" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D83" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B84" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D84" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D85" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>189</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>188</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="C86" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D86" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>192</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C87" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D87" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>195</v>
-      </c>
-      <c r="B87" t="s">
-        <v>194</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D87" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B88" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D88" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D89" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D90" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D91" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B92" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D92" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B93" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D93" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D94" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B95" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B96" t="s">
-        <v>221</v>
-      </c>
-      <c r="C96" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D96" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B97" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C97" t="s">
         <v>571</v>
       </c>
       <c r="D97" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B98" t="s">
-        <v>227</v>
-      </c>
-      <c r="C98" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C98" t="s">
         <v>571</v>
       </c>
       <c r="D98" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B99" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D99" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B100" t="s">
-        <v>232</v>
-      </c>
-      <c r="C100" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D100" t="s">
-        <v>562</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B101" t="s">
-        <v>235</v>
-      </c>
-      <c r="C101" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" t="s">
         <v>571</v>
       </c>
       <c r="D101" t="s">
-        <v>234</v>
+        <v>562</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B102" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D102" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B103" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D103" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B104" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D104" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B105" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D105" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B106" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D106" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B107" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D107" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B108" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D108" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B109" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D109" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>612</v>
+        <v>260</v>
       </c>
       <c r="B110" t="s">
-        <v>613</v>
+        <v>259</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D110" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>263</v>
+        <v>612</v>
       </c>
       <c r="B111" t="s">
-        <v>262</v>
+        <v>613</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D111" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B112" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D112" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B113" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D113" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B114" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D114" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B115" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D115" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B116" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D116" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B117" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D117" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B118" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D118" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D119" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B120" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D120" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B121" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D121" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B122" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D122" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B123" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D123" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>614</v>
+        <v>297</v>
       </c>
       <c r="B124" t="s">
-        <v>615</v>
+        <v>296</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D124" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>300</v>
+        <v>614</v>
       </c>
       <c r="B125" t="s">
-        <v>299</v>
+        <v>615</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D125" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B126" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D126" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B127" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D127" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B128" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D128" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B129" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D129" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B130" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D130" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B131" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D131" t="s">
-        <v>563</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B132" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D132" t="s">
-        <v>317</v>
+        <v>563</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B133" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D133" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B134" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D134" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B135" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D135" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B136" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D136" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B137" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D137" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B138" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D138" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B139" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D139" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B140" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D140" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B141" t="s">
-        <v>344</v>
-      </c>
-      <c r="C141" t="s">
-        <v>571</v>
-      </c>
-      <c r="D141" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B142" t="s">
-        <v>347</v>
-      </c>
-      <c r="C142" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C142" t="s">
         <v>571</v>
       </c>
       <c r="D142" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B143" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D143" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B144" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D144" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B145" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D145" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B146" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D146" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>616</v>
+        <v>360</v>
       </c>
       <c r="B147" t="s">
-        <v>617</v>
+        <v>359</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D147" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>363</v>
+        <v>616</v>
       </c>
       <c r="B148" t="s">
-        <v>362</v>
+        <v>617</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D148" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B149" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D149" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B150" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D150" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B151" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D151" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B152" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D152" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B153" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D153" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B154" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D154" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B155" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D155" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B156" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D156" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B157" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D157" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B158" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D158" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B159" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D159" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>395</v>
+      </c>
+      <c r="B160" t="s">
+        <v>394</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D160" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>398</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>397</v>
       </c>
-      <c r="C160" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D160" t="s">
+      <c r="C161" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D161" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="162" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>400</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" t="s">
         <v>399</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D161" s="2" t="s">
+      <c r="C162" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D162" s="2" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>602</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>618</v>
-      </c>
-      <c r="B163" t="s">
-        <v>619</v>
+        <v>602</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>603</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>571</v>
@@ -4515,10 +4521,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B164" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>571</v>
@@ -4526,10 +4532,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B165" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>571</v>
@@ -4537,10 +4543,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B166" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>571</v>
@@ -4548,10 +4554,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B167" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>571</v>
@@ -4559,10 +4565,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B168" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>571</v>
@@ -4570,10 +4576,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B169" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>571</v>
@@ -4581,10 +4587,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B170" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>571</v>
@@ -4592,10 +4598,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B171" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>571</v>
@@ -4603,10 +4609,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B172" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>571</v>
@@ -4614,58 +4620,55 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>402</v>
+        <v>636</v>
       </c>
       <c r="B173" t="s">
-        <v>401</v>
+        <v>637</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D173" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B174" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D174" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B175" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D175" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B176" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D176" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4679,264 +4682,267 @@
         <v>571</v>
       </c>
       <c r="D177" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B178" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D178" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B179" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D179" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B180" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D180" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B181" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D181" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B182" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D182" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B183" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D183" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B184" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D184" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B185" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D185" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B186" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D186" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B187" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D187" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B188" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D188" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B189" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D189" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B190" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D190" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B191" t="s">
-        <v>453</v>
-      </c>
-      <c r="C191" t="s">
+        <v>450</v>
+      </c>
+      <c r="C191" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D191" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B192" t="s">
-        <v>456</v>
-      </c>
-      <c r="C192" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C192" t="s">
         <v>571</v>
       </c>
       <c r="D192" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B193" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D193" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B194" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D194" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B195" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D195" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B196" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>571</v>
@@ -4944,10 +4950,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B197" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>571</v>
@@ -4955,102 +4961,102 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B198" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D198" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B199" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D199" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B200" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D200" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B201" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D201" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B202" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D202" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B203" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D203" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B204" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D204" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B205" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>571</v>
@@ -5058,271 +5064,271 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B206" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D206" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B207" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D207" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B208" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D208" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B209" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D209" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B210" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D210" t="s">
-        <v>565</v>
-      </c>
-      <c r="E210" t="s">
-        <v>571</v>
+        <v>499</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B211" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D211" t="s">
-        <v>504</v>
+        <v>565</v>
+      </c>
+      <c r="E211" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B212" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D212" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B213" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D213" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B214" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D214" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B215" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D215" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B216" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D216" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B217" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D217" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B218" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D218" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B219" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D219" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>529</v>
+      </c>
+      <c r="B220" t="s">
+        <v>528</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D220" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
         <v>532</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B221" t="s">
         <v>531</v>
       </c>
-      <c r="C220" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D220" t="s">
+      <c r="C221" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D221" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="222" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>534</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>533</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D221" s="1"/>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>537</v>
-      </c>
-      <c r="B222" t="s">
-        <v>536</v>
-      </c>
       <c r="C222" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D222" t="s">
-        <v>535</v>
-      </c>
+      <c r="D222" s="1"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B223" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D223" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B224" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D224" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B225" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>571</v>
@@ -5330,107 +5336,118 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B226" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D226" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>594</v>
+        <v>547</v>
       </c>
       <c r="B227" t="s">
-        <v>595</v>
+        <v>546</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="E227" t="s">
-        <v>571</v>
+      <c r="D227" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>550</v>
+        <v>594</v>
       </c>
       <c r="B228" t="s">
-        <v>549</v>
+        <v>595</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D228" t="s">
-        <v>548</v>
+      <c r="E228" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B229" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D229" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>639</v>
+        <v>553</v>
       </c>
       <c r="B230" t="s">
-        <v>638</v>
+        <v>552</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D230" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
+        <v>639</v>
+      </c>
+      <c r="B231" t="s">
+        <v>638</v>
+      </c>
+      <c r="C231" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
         <v>556</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>555</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D231" t="s">
+      <c r="C232" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D232" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
+    <row r="233" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>559</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B233" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D232" t="s">
+      <c r="C233" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D233" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A233" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
         <v>574</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>575</v>
       </c>
-      <c r="C233" s="4" t="s">
+      <c r="C234" s="4" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import 3 OBCS software terms   added in the ontoFox OBO input file, however, manually import in since the terms in development version of OBCS now import IAO:written name   added in both ontoFox and ontoDog input files, current import via ontoFox import VIVO-ISF, dataProperty: first name, last name   added manually
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="644">
   <si>
     <t>planned process</t>
   </si>
@@ -1942,6 +1942,12 @@
   </si>
   <si>
     <t>transcription factor binding site  identification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000590</t>
+  </si>
+  <si>
+    <t>written name</t>
   </si>
 </sst>
 </file>
@@ -2312,10 +2318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2478,253 +2484,253 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>642</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>643</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D14" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>609</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>608</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>609</v>
+      </c>
+      <c r="B23" t="s">
+        <v>608</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D25" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>606</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>607</v>
+        <v>29</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="E26" t="s">
-        <v>571</v>
+      <c r="D26" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>606</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>607</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D27" t="s">
-        <v>31</v>
+      <c r="E27" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>640</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>641</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>571</v>
@@ -2732,63 +2738,63 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>640</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>641</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D33" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>610</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>611</v>
+        <v>53</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>571</v>
@@ -2796,10 +2802,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>610</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>611</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>571</v>
@@ -2807,10 +2813,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>571</v>
@@ -2818,44 +2824,41 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D40" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2868,1663 +2871,1666 @@
       <c r="C43" s="4" t="s">
         <v>571</v>
       </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D44" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>593</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>592</v>
+        <v>84</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>591</v>
+      <c r="D50" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>600</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>601</v>
+        <v>593</v>
+      </c>
+      <c r="B51" t="s">
+        <v>592</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" t="s">
-        <v>87</v>
+        <v>600</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>601</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D52" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D53" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>111</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>110</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C61" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D61" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C62" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D62" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D62" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D64" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D65" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D66" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D68" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D70" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D71" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D72" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D73" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D74" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D75" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D76" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>162</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>161</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="C78" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D78" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>165</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C79" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D79" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>168</v>
-      </c>
-      <c r="B79" t="s">
-        <v>167</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D79" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D80" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B81" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D82" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D83" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B84" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D84" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D85" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>186</v>
+      </c>
+      <c r="B86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D86" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>189</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>188</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C87" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D87" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>192</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C88" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D88" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>195</v>
-      </c>
-      <c r="B88" t="s">
-        <v>194</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D88" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B89" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D89" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B90" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D90" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B91" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D91" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B92" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D92" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B93" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D93" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B94" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D94" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B95" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D95" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D96" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B97" t="s">
-        <v>221</v>
-      </c>
-      <c r="C97" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D97" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B98" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C98" t="s">
         <v>571</v>
       </c>
       <c r="D98" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B99" t="s">
-        <v>227</v>
-      </c>
-      <c r="C99" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C99" t="s">
         <v>571</v>
       </c>
       <c r="D99" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B100" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D100" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B101" t="s">
-        <v>232</v>
-      </c>
-      <c r="C101" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D101" t="s">
-        <v>562</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B102" t="s">
-        <v>235</v>
-      </c>
-      <c r="C102" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C102" t="s">
         <v>571</v>
       </c>
       <c r="D102" t="s">
-        <v>234</v>
+        <v>562</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D103" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B104" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D104" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B105" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D105" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B106" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D106" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B107" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D107" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B108" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D108" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B109" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D109" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B110" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D110" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>612</v>
+        <v>260</v>
       </c>
       <c r="B111" t="s">
-        <v>613</v>
+        <v>259</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D111" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>263</v>
+        <v>612</v>
       </c>
       <c r="B112" t="s">
-        <v>262</v>
+        <v>613</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D112" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B113" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D113" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B114" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D114" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D115" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B116" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D116" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B117" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D117" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B118" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D118" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B119" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D119" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B120" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D120" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B121" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D121" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B122" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D122" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B123" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D123" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B124" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D124" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>614</v>
+        <v>297</v>
       </c>
       <c r="B125" t="s">
-        <v>615</v>
+        <v>296</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D125" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>300</v>
+        <v>614</v>
       </c>
       <c r="B126" t="s">
-        <v>299</v>
+        <v>615</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D126" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B127" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D127" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B128" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D128" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B129" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D129" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B130" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D130" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B131" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D131" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B132" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D132" t="s">
-        <v>563</v>
+        <v>312</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D133" t="s">
-        <v>317</v>
+        <v>563</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B134" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D134" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B135" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D135" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B136" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D136" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B137" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D137" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B138" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D138" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B139" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D139" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B140" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D140" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B141" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D141" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B142" t="s">
-        <v>344</v>
-      </c>
-      <c r="C142" t="s">
-        <v>571</v>
-      </c>
-      <c r="D142" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
-        <v>347</v>
-      </c>
-      <c r="C143" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C143" t="s">
         <v>571</v>
       </c>
       <c r="D143" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B144" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D144" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B145" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D145" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B146" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D146" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B147" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D147" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>616</v>
+        <v>360</v>
       </c>
       <c r="B148" t="s">
-        <v>617</v>
+        <v>359</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D148" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>363</v>
+        <v>616</v>
       </c>
       <c r="B149" t="s">
-        <v>362</v>
+        <v>617</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D149" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B150" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D150" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B151" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D151" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B152" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D152" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B153" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D153" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B154" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D154" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B155" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D155" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B156" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D156" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B157" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D157" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B158" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D158" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B159" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D159" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B160" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D160" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>395</v>
+      </c>
+      <c r="B161" t="s">
+        <v>394</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D161" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>398</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" t="s">
         <v>397</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D161" t="s">
+      <c r="C162" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D162" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="163" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>400</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>399</v>
       </c>
-      <c r="C162" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D162" s="2" t="s">
+      <c r="C163" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D163" s="2" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>602</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>618</v>
-      </c>
-      <c r="B164" t="s">
-        <v>619</v>
+        <v>602</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>603</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>571</v>
@@ -4532,10 +4538,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B165" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>571</v>
@@ -4543,10 +4549,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B166" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>571</v>
@@ -4554,10 +4560,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B167" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>571</v>
@@ -4565,10 +4571,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B168" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>571</v>
@@ -4576,10 +4582,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B169" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>571</v>
@@ -4587,10 +4593,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B170" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>571</v>
@@ -4598,10 +4604,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B171" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>571</v>
@@ -4609,10 +4615,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B172" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>571</v>
@@ -4620,10 +4626,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B173" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>571</v>
@@ -4631,58 +4637,55 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>402</v>
+        <v>636</v>
       </c>
       <c r="B174" t="s">
-        <v>401</v>
+        <v>637</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D174" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B175" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D175" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B176" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D176" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B177" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D177" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -4696,264 +4699,267 @@
         <v>571</v>
       </c>
       <c r="D178" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B179" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D179" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B180" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D180" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B181" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D181" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B182" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D182" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B183" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D183" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B184" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D184" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B185" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D185" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B186" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D186" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B187" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D187" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B188" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D188" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B189" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D189" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B190" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D190" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B191" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D191" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B192" t="s">
-        <v>453</v>
-      </c>
-      <c r="C192" t="s">
+        <v>450</v>
+      </c>
+      <c r="C192" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D192" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B193" t="s">
-        <v>456</v>
-      </c>
-      <c r="C193" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C193" t="s">
         <v>571</v>
       </c>
       <c r="D193" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B194" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D194" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B195" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D195" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B196" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D196" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B197" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>571</v>
@@ -4961,10 +4967,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B198" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>571</v>
@@ -4972,102 +4978,102 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B199" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D199" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B200" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D200" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B201" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D201" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B202" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D202" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B203" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D203" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B204" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D204" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B205" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D205" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B206" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>571</v>
@@ -5075,271 +5081,271 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B207" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D207" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B208" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D208" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B209" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D209" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B210" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D210" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B211" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D211" t="s">
-        <v>565</v>
-      </c>
-      <c r="E211" t="s">
-        <v>571</v>
+        <v>499</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B212" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D212" t="s">
-        <v>504</v>
+        <v>565</v>
+      </c>
+      <c r="E212" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B213" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D213" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B214" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D214" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B215" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D215" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B216" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D216" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B217" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D217" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B218" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D218" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B219" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D219" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B220" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D220" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>529</v>
+      </c>
+      <c r="B221" t="s">
+        <v>528</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D221" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
         <v>532</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>531</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D221" t="s">
+      <c r="C222" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D222" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="223" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>534</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" t="s">
         <v>533</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D222" s="1"/>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
-        <v>537</v>
-      </c>
-      <c r="B223" t="s">
-        <v>536</v>
-      </c>
       <c r="C223" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D223" t="s">
-        <v>535</v>
-      </c>
+      <c r="D223" s="1"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B224" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D224" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B225" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D225" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B226" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>571</v>
@@ -5347,107 +5353,118 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B227" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="D227" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>594</v>
+        <v>547</v>
       </c>
       <c r="B228" t="s">
-        <v>595</v>
+        <v>546</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="E228" t="s">
-        <v>571</v>
+      <c r="D228" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>550</v>
+        <v>594</v>
       </c>
       <c r="B229" t="s">
-        <v>549</v>
+        <v>595</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="D229" t="s">
-        <v>548</v>
+      <c r="E229" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B230" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>571</v>
       </c>
       <c r="D230" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>639</v>
+        <v>553</v>
       </c>
       <c r="B231" t="s">
-        <v>638</v>
+        <v>552</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>571</v>
+      </c>
+      <c r="D231" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>639</v>
+      </c>
+      <c r="B232" t="s">
+        <v>638</v>
+      </c>
+      <c r="C232" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
         <v>556</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>555</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D232" t="s">
+      <c r="C233" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D233" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+    <row r="234" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>559</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B234" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C233" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="D233" t="s">
+      <c r="C234" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="D234" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A234" t="s">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
         <v>574</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>575</v>
       </c>
-      <c r="C234" s="4" t="s">
+      <c r="C235" s="4" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add OBI:'gene list' that should be imported into BCGO
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="646">
   <si>
     <t>planned process</t>
   </si>
@@ -1948,6 +1948,12 @@
   </si>
   <si>
     <t>written name</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000118</t>
+  </si>
+  <si>
+    <t>gene list</t>
   </si>
 </sst>
 </file>
@@ -2318,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E235"/>
+  <dimension ref="A1:E236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5465,6 +5471,17 @@
         <v>575</v>
       </c>
       <c r="C235" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>644</v>
+      </c>
+      <c r="B236" t="s">
+        <v>645</v>
+      </c>
+      <c r="C236" s="4" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add three terms of study design variables need for BCBC studies
</commit_message>
<xml_diff>
--- a/doc/Ontodog/OBI_input.xlsx
+++ b/doc/Ontodog/OBI_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="652">
   <si>
     <t>planned process</t>
   </si>
@@ -1954,6 +1954,24 @@
   </si>
   <si>
     <t>gene list</t>
+  </si>
+  <si>
+    <t>study design controlled variable</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000785</t>
+  </si>
+  <si>
+    <t>study design dependent variable</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000751</t>
+  </si>
+  <si>
+    <t>study design independent variable</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000750</t>
   </si>
 </sst>
 </file>
@@ -2324,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E236"/>
+  <dimension ref="A1:E239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C240" sqref="C240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5482,6 +5500,39 @@
         <v>645</v>
       </c>
       <c r="C236" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>647</v>
+      </c>
+      <c r="B237" t="s">
+        <v>646</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>649</v>
+      </c>
+      <c r="B238" t="s">
+        <v>648</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>651</v>
+      </c>
+      <c r="B239" t="s">
+        <v>650</v>
+      </c>
+      <c r="C239" s="4" t="s">
         <v>571</v>
       </c>
     </row>

</xml_diff>